<commit_message>
minor updates on styling
</commit_message>
<xml_diff>
--- a/ATGScrape/insider_event.xlsx
+++ b/ATGScrape/insider_event.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raosa\Documents\ATG-WebScraping\ATGScrape\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3509CE20-BD60-4CFD-8E89-AAACF61638C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="62">
   <si>
     <t>EVENT NAME</t>
   </si>
@@ -49,9 +43,15 @@
     <t xml:space="preserve">Groom. Enhance. Transform </t>
   </si>
   <si>
+    <t>Illusionary Line Art Workshop</t>
+  </si>
+  <si>
     <t>Jhumritalaiya - Online Storytelling Mentorship Program</t>
   </si>
   <si>
+    <t>Learn Mandala Art - A One Page Spotlight Workshop</t>
+  </si>
+  <si>
     <t>Lose 3 Kgs in 30 Days, by Masterlife.</t>
   </si>
   <si>
@@ -61,6 +61,9 @@
     <t>MyCaptain Tech Wizard</t>
   </si>
   <si>
+    <t>Online Internship Program for Drone/Robotics/IoT/Computer Vision</t>
+  </si>
+  <si>
     <t>Online Program in Direction by WWI Virtual Academy</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t>Online Program in Screenwriting by WWI Virtual Academy</t>
   </si>
   <si>
+    <t>Paper Mache [Online Live Workshop - Inclusive of Materials]</t>
+  </si>
+  <si>
     <t>SHARAN 21- Day Online Diabetes Reversal Program</t>
   </si>
   <si>
@@ -91,9 +97,15 @@
     <t>December 14 | 12PM - December 21 | 1PM</t>
   </si>
   <si>
+    <t>December 19 | 3PM</t>
+  </si>
+  <si>
     <t>6 Sessions | Choose your own Schedule!</t>
   </si>
   <si>
+    <t>September 27 | 12PM - December 31 | 6PM</t>
+  </si>
+  <si>
     <t>Everyday | 2PM</t>
   </si>
   <si>
@@ -103,9 +115,15 @@
     <t>July 1 - 30 | 8:30PM</t>
   </si>
   <si>
+    <t>August 21 | 10AM - December 31 | 4PM</t>
+  </si>
+  <si>
     <t>Access to online course material for a year.</t>
   </si>
   <si>
+    <t>December 19 | 11AM</t>
+  </si>
+  <si>
     <t>September 29 | 10:30AM - November 30 | 10:00PM</t>
   </si>
   <si>
@@ -127,6 +145,9 @@
     <t>4500</t>
   </si>
   <si>
+    <t>150</t>
+  </si>
+  <si>
     <t>5999</t>
   </si>
   <si>
@@ -136,21 +157,24 @@
     <t>3500</t>
   </si>
   <si>
+    <t>1000</t>
+  </si>
+  <si>
     <t>13000</t>
   </si>
   <si>
     <t>9000</t>
   </si>
   <si>
+    <t>1500 onwards</t>
+  </si>
+  <si>
     <t>1475 onwards</t>
   </si>
   <si>
     <t>9440</t>
   </si>
   <si>
-    <t>1500 onwards</t>
-  </si>
-  <si>
     <t>Online</t>
   </si>
   <si>
@@ -160,6 +184,12 @@
     <t>Your Home</t>
   </si>
   <si>
+    <t>To Be Announced</t>
+  </si>
+  <si>
+    <t>Zoom Call</t>
+  </si>
+  <si>
     <t>Watch on Zoom</t>
   </si>
   <si>
@@ -167,13 +197,16 @@
   </si>
   <si>
     <t>online-skill</t>
+  </si>
+  <si>
+    <t>online-hobby</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -236,14 +269,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -290,7 +315,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,27 +347,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -374,24 +381,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,23 +556,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="48.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,242 +580,310 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="E6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D10" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E15" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>